<commit_message>
S3-03b HK — Importers: seed as GLOBAL (org_id NULL) + new Materials seed path
- import_materials.py: add org_id to INSERT (global), update seed default to data/Materials_DB_Seed.xlsx,
  prepend NULL org_id to tuples, keep is_active, count only global rows in logs.
- import_dje_items.py: add org_id to INSERT (global), prepend NULL org_id to tuples,
  keep is_active, count only global rows in logs.

Note: conflict targets unchanged (still partial on is_active) to avoid migration churn today.
</commit_message>
<xml_diff>
--- a/data/dje_items.xlsx
+++ b/data/dje_items.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharm\Desktop\electrical-estimator\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sharm\code\electrical-estimator-saas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC941BF5-5AC5-43EB-9A4A-D204D8427DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2970570E-0CF1-464B-8BF6-A85E57B4D791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E91AC5E7-6D22-4E0A-9016-3C40061F3CC7}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <definedName name="Branch_List">'[1]Labor Adj &amp; Multi'!$V$2:$V$6</definedName>
     <definedName name="Categories">_xlfn.ANCHORARRAY('[1]Labor Adj &amp; Multi'!$AD$2)</definedName>
     <definedName name="DV_Items">'[1]Labor Adj &amp; Multi'!$AF$2:$AF$55</definedName>
-    <definedName name="FullList">'Labor Unit &amp; Material Pricing'!$D$2:$D$40</definedName>
+    <definedName name="FullList">'Labor Unit &amp; Material Pricing'!$D$2:$D$39</definedName>
     <definedName name="qqfxlBookName" hidden="1">"ETB VBA Material Test rev3.1.1.xlsm"</definedName>
     <definedName name="qqfxlNamesRange" hidden="1">#REF!</definedName>
   </definedNames>
@@ -47,13 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="102">
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>DJE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="59">
   <si>
     <t>Enviromental</t>
   </si>
@@ -187,126 +181,6 @@
     <t>Parking</t>
   </si>
   <si>
-    <t>Added Cushion</t>
-  </si>
-  <si>
-    <t>DJE-000001</t>
-  </si>
-  <si>
-    <t>DJE-000002</t>
-  </si>
-  <si>
-    <t>DJE-000003</t>
-  </si>
-  <si>
-    <t>DJE-000004</t>
-  </si>
-  <si>
-    <t>DJE-000005</t>
-  </si>
-  <si>
-    <t>DJE-000006</t>
-  </si>
-  <si>
-    <t>DJE-000007</t>
-  </si>
-  <si>
-    <t>DJE-000008</t>
-  </si>
-  <si>
-    <t>DJE-000009</t>
-  </si>
-  <si>
-    <t>DJE-000010</t>
-  </si>
-  <si>
-    <t>DJE-000011</t>
-  </si>
-  <si>
-    <t>DJE-000012</t>
-  </si>
-  <si>
-    <t>DJE-000013</t>
-  </si>
-  <si>
-    <t>DJE-000014</t>
-  </si>
-  <si>
-    <t>DJE-000015</t>
-  </si>
-  <si>
-    <t>DJE-000016</t>
-  </si>
-  <si>
-    <t>DJE-000017</t>
-  </si>
-  <si>
-    <t>DJE-000018</t>
-  </si>
-  <si>
-    <t>DJE-000019</t>
-  </si>
-  <si>
-    <t>DJE-000020</t>
-  </si>
-  <si>
-    <t>DJE-000021</t>
-  </si>
-  <si>
-    <t>DJE-000022</t>
-  </si>
-  <si>
-    <t>DJE-000023</t>
-  </si>
-  <si>
-    <t>DJE-000024</t>
-  </si>
-  <si>
-    <t>DJE-000025</t>
-  </si>
-  <si>
-    <t>DJE-000026</t>
-  </si>
-  <si>
-    <t>DJE-000027</t>
-  </si>
-  <si>
-    <t>DJE-000028</t>
-  </si>
-  <si>
-    <t>DJE-000029</t>
-  </si>
-  <si>
-    <t>DJE-000030</t>
-  </si>
-  <si>
-    <t>DJE-000031</t>
-  </si>
-  <si>
-    <t>DJE-000032</t>
-  </si>
-  <si>
-    <t>DJE-000033</t>
-  </si>
-  <si>
-    <t>DJE-000034</t>
-  </si>
-  <si>
-    <t>DJE-000035</t>
-  </si>
-  <si>
-    <t>DJE-000036</t>
-  </si>
-  <si>
-    <t>DJE-000037</t>
-  </si>
-  <si>
-    <t>DJE-000038</t>
-  </si>
-  <si>
-    <t>DJE-000039</t>
-  </si>
-  <si>
     <t>Fees</t>
   </si>
   <si>
@@ -319,9 +193,6 @@
     <t>Office</t>
   </si>
   <si>
-    <t>Cushion</t>
-  </si>
-  <si>
     <t>Hotel</t>
   </si>
   <si>
@@ -334,9 +205,6 @@
     <t>Parking/Tolls/Drivetime</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -353,6 +221,9 @@
   </si>
   <si>
     <t>cost_code</t>
+  </si>
+  <si>
+    <t>is_active</t>
   </si>
 </sst>
 </file>
@@ -430,7 +301,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="9">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -445,9 +316,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -811,17 +679,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02A2D01B-D2FA-47FB-BF70-69CFFFB95076}" name="Database" displayName="Database" ref="A1:H40" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H40" xr:uid="{641F3A69-F920-4D14-9E98-8686467851EB}"/>
-  <tableColumns count="8">
-    <tableColumn id="13" xr3:uid="{C2F6B7AF-12FD-4E3C-9311-C80C4EF5A4EA}" name="id" dataDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{AA583652-70CF-4842-9468-F2D6F5106868}" name="category" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{DB956E10-BC9F-44D2-A939-C82E79317A16}" name="subcategory" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02A2D01B-D2FA-47FB-BF70-69CFFFB95076}" name="Database" displayName="Database" ref="A1:G39" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G39" xr:uid="{641F3A69-F920-4D14-9E98-8686467851EB}"/>
+  <tableColumns count="7">
+    <tableColumn id="13" xr3:uid="{C2F6B7AF-12FD-4E3C-9311-C80C4EF5A4EA}" name="is_active" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{AA583652-70CF-4842-9468-F2D6F5106868}" name="category" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{DB956E10-BC9F-44D2-A939-C82E79317A16}" name="subcategory" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{9E75E4FC-3F39-4444-85B3-398028FCE0BC}" name="description" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{22AD6D15-EA41-4AB7-9408-02E4418271AE}" name="default_unit_cost" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{69D3BD58-F791-4673-B4AE-BB4C9F31A307}" name="Unit" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{4D29D692-FAFA-4618-94F1-FF89EEF8EC29}" name="vendor" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{6C93A415-50BB-4CB0-8C1C-3B6ACCD59D3E}" name="cost_code" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{4D29D692-FAFA-4618-94F1-FF89EEF8EC29}" name="vendor" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{6C93A415-50BB-4CB0-8C1C-3B6ACCD59D3E}" name="cost_code" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1093,909 +960,770 @@
   <sheetPr codeName="Sheet16">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:H2937"/>
+  <dimension ref="A1:G2936"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" style="6" customWidth="1"/>
     <col min="2" max="3" width="30.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="209.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="24" style="6" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="4" width="54.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="24" style="6" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>95</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
       </c>
       <c r="E2" s="5">
         <v>7.5</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" s="5">
         <v>85</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" s="5">
         <v>85</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5" s="5">
         <v>145</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="b">
         <v>1</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="E6" s="5">
         <v>275</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7" s="5">
         <v>335</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5">
         <v>195</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="b">
         <v>1</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="5">
         <v>510</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="b">
         <v>1</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10" s="5">
         <v>850</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="b">
         <v>1</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="B11" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E11" s="5">
         <v>250</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="b">
         <v>1</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="E12" s="5">
         <v>865</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="b">
         <v>1</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E13" s="5">
         <v>1600</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="b">
         <v>1</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="B14" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14" s="5">
         <v>700</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="b">
         <v>1</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="B15" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E15" s="5">
         <v>1800</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="b">
         <v>1</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E16" s="5">
         <v>3600</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="b">
         <v>1</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E17" s="5">
         <v>285</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="b">
         <v>1</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="E18" s="5">
         <v>995</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="b">
         <v>1</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="B19" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E19" s="5">
         <v>2150</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="b">
         <v>1</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="B20" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E20" s="5">
         <v>245</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="b">
         <v>1</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="B21" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E21" s="5">
         <v>1200</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="b">
         <v>1</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="B22" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E22" s="5">
         <v>2560</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="b">
         <v>1</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="B23" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E23" s="5">
         <v>550</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="b">
         <v>1</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="B24" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E24" s="5">
         <v>1920</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="b">
         <v>1</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="B25" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E25" s="5">
         <v>3820</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="b">
         <v>1</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="B26" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E26" s="5">
         <v>145</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="b">
         <v>1</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="B27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="E27" s="5">
         <v>179</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="b">
         <v>1</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="B28" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E28" s="5">
         <v>650</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="b">
         <v>1</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="B29" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E29" s="5">
         <v>850</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="b">
         <v>1</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="B30" s="4" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E30" s="5">
         <v>50</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="b">
         <v>1</v>
       </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="B31" s="4" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="C31" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="E31" s="5">
         <v>75</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="b">
         <v>1</v>
       </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="B32" s="4" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E32" s="5">
         <v>125</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="b">
         <v>1</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="B33" s="4" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E33" s="5">
         <v>50</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="b">
         <v>1</v>
       </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="B34" s="4" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E34" s="5">
         <v>150</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="b">
         <v>1</v>
       </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="B35" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="E35" s="5">
         <v>150</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="b">
         <v>1</v>
       </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="B36" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E36" s="5">
         <v>1.25</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="b">
         <v>1</v>
       </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="B37" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="E37" s="5">
         <v>50</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="b">
         <v>1</v>
       </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="B38" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E38" s="5">
         <v>4</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="b">
         <v>1</v>
       </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="B39" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E39" s="5">
         <v>50</v>
       </c>
-      <c r="F39" s="4">
-        <v>1</v>
-      </c>
+      <c r="F39" s="4"/>
       <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E40" s="5">
-        <v>1000</v>
-      </c>
-      <c r="F40" s="4">
-        <v>1</v>
-      </c>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-    </row>
+    <row r="50" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="51" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="52" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="53" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4882,11 +4610,10 @@
     <row r="2934" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2935" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2936" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2937" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection sort="0" autoFilter="0"/>
   <protectedRanges>
-    <protectedRange sqref="H1" name="AllowMaterialLaborSortFilter"/>
+    <protectedRange sqref="G1" name="AllowMaterialLaborSortFilter"/>
   </protectedRanges>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>